<commit_message>
Add CVSD sound board files and plan rom layout
</commit_message>
<xml_diff>
--- a/doc/rom_calc_joust2.xlsx
+++ b/doc/rom_calc_joust2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Arcade-Joust2_MiSTer\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kcoleman\Documents\GitHub\Arcade-Joust2_MiSTer\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A54E3A-1135-49A6-8B50-1C85E193118F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00F1364-2A3A-4697-820F-ED052395E303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14550" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ROM Map" sheetId="2" r:id="rId1"/>
@@ -32,10 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="115">
-  <si>
-    <t>MAME</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="115">
   <si>
     <t>section</t>
   </si>
@@ -49,9 +46,6 @@
     <t>size</t>
   </si>
   <si>
-    <t>gfx1</t>
-  </si>
-  <si>
     <t>joust2_graph1</t>
   </si>
   <si>
@@ -70,9 +64,6 @@
     <t>vid_27128_ic41_rom22_rev1.9d</t>
   </si>
   <si>
-    <t>maincpu</t>
-  </si>
-  <si>
     <t>joust2_bank_a</t>
   </si>
   <si>
@@ -130,9 +121,6 @@
     <t>cpu_2732_ic13_rom6_rev2.6i</t>
   </si>
   <si>
-    <t>soundcpu</t>
-  </si>
-  <si>
     <t>joust2_sound</t>
   </si>
   <si>
@@ -172,9 +160,6 @@
     <t>vid_82s123_ic14_a-5282-10295.2b</t>
   </si>
   <si>
-    <t>bg:cpu</t>
-  </si>
-  <si>
     <t>snd_27256_rom23_rev1.u4</t>
   </si>
   <si>
@@ -253,33 +238,15 @@
     <t>0ea3f7fb</t>
   </si>
   <si>
-    <t>17:14</t>
-  </si>
-  <si>
-    <t>17:12</t>
-  </si>
-  <si>
-    <t>17:13</t>
-  </si>
-  <si>
     <t>Bitrange</t>
   </si>
   <si>
     <t>BLANK</t>
   </si>
   <si>
-    <t>0001</t>
-  </si>
-  <si>
     <t>0010</t>
   </si>
   <si>
-    <t>0000</t>
-  </si>
-  <si>
-    <t>17:9</t>
-  </si>
-  <si>
     <t>bitpattern end</t>
   </si>
   <si>
@@ -301,33 +268,9 @@
     <t>Size</t>
   </si>
   <si>
-    <t>17:15</t>
-  </si>
-  <si>
-    <t>010</t>
-  </si>
-  <si>
-    <t>011</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>101</t>
-  </si>
-  <si>
-    <t>11100</t>
-  </si>
-  <si>
-    <t>11000</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>11001</t>
-  </si>
-  <si>
     <t>d'Start</t>
   </si>
   <si>
@@ -340,15 +283,9 @@
     <t>padding</t>
   </si>
   <si>
-    <t>11011</t>
-  </si>
-  <si>
     <t>expand to 32kb</t>
   </si>
   <si>
-    <t>111110</t>
-  </si>
-  <si>
     <t>13:0</t>
   </si>
   <si>
@@ -364,19 +301,82 @@
     <t>8:0</t>
   </si>
   <si>
-    <t>111101</t>
-  </si>
-  <si>
-    <t>111111000</t>
-  </si>
-  <si>
     <t>Corebits</t>
   </si>
   <si>
-    <t>testing prog2 for regression now</t>
-  </si>
-  <si>
     <t>bitpattern start</t>
+  </si>
+  <si>
+    <t>3AF6B47D</t>
+  </si>
+  <si>
+    <t>E7F9ED2E</t>
+  </si>
+  <si>
+    <t>C85B29F7</t>
+  </si>
+  <si>
+    <t>18:14</t>
+  </si>
+  <si>
+    <t>18:15</t>
+  </si>
+  <si>
+    <t>00000</t>
+  </si>
+  <si>
+    <t>00001</t>
+  </si>
+  <si>
+    <t>00010</t>
+  </si>
+  <si>
+    <t>00011</t>
+  </si>
+  <si>
+    <t>0110</t>
+  </si>
+  <si>
+    <t>0111</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>0100</t>
+  </si>
+  <si>
+    <t>0101</t>
+  </si>
+  <si>
+    <t>18:13</t>
+  </si>
+  <si>
+    <t>18:12</t>
+  </si>
+  <si>
+    <t>18:9</t>
+  </si>
+  <si>
+    <t>100100</t>
+  </si>
+  <si>
+    <t>100101</t>
+  </si>
+  <si>
+    <t>100110</t>
+  </si>
+  <si>
+    <t>1001101000</t>
+  </si>
+  <si>
+    <t>sound_bank_a</t>
+  </si>
+  <si>
+    <t>sound_bank_b</t>
+  </si>
+  <si>
+    <t>sound_bank_c</t>
   </si>
 </sst>
 </file>
@@ -438,7 +438,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -449,6 +449,36 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFCCCCCC"/>
         <bgColor rgb="FFCCCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -508,7 +538,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -566,6 +596,107 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -815,10 +946,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47A4B22B-6618-4C49-8781-19881A3A2D30}">
-  <dimension ref="A1:P36"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -832,57 +963,55 @@
     <col min="9" max="9" width="9" style="1" customWidth="1"/>
     <col min="10" max="11" width="29" style="1" customWidth="1"/>
     <col min="12" max="12" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="3"/>
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>4</v>
-      </c>
       <c r="F1" s="5" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -903,17 +1032,15 @@
       <c r="O2" s="14"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="7"/>
+      <c r="B3" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>7</v>
-      </c>
       <c r="D3" s="17" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E3" s="18">
         <v>16384</v>
@@ -943,30 +1070,28 @@
         <v>000000000000000000000000</v>
       </c>
       <c r="L3" s="21" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="M3" s="22" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="N3" s="28" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="O3" s="20" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="A4" s="7"/>
       <c r="B4" s="17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E4" s="18">
         <v>16384</v>
@@ -996,30 +1121,28 @@
         <v>000000000100000000000000</v>
       </c>
       <c r="L4" s="21" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="M4" s="22" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="N4" s="28" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="O4" s="20" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="A5" s="7"/>
       <c r="B5" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E5" s="18">
         <v>16384</v>
@@ -1049,25 +1172,25 @@
         <v>000000001000000000000000</v>
       </c>
       <c r="L5" s="21" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="M5" s="22" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="N5" s="28" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="O5" s="20" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="17" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="18">
@@ -1098,857 +1221,823 @@
         <v>000000001100000000000000</v>
       </c>
       <c r="L6" s="21" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="M6" s="22" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="N6" s="28" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="O6" s="20" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" s="18">
+      <c r="A7" s="62"/>
+      <c r="B7" s="62" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="62" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="62" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="63">
         <v>8192</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="63">
         <f t="shared" si="0"/>
         <v>65536</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="63">
         <f t="shared" si="1"/>
         <v>73727</v>
       </c>
-      <c r="H7" s="26" t="str">
+      <c r="H7" s="64" t="str">
         <f t="shared" si="3"/>
         <v>10000</v>
       </c>
-      <c r="I7" s="27" t="str">
+      <c r="I7" s="65" t="str">
         <f t="shared" si="4"/>
         <v>11FFF</v>
       </c>
-      <c r="J7" s="20" t="str">
+      <c r="J7" s="66" t="str">
         <f t="shared" si="5"/>
         <v>000000010001111111111111</v>
       </c>
-      <c r="K7" s="20" t="str">
+      <c r="K7" s="66" t="str">
         <f t="shared" si="2"/>
         <v>000000010000000000000000</v>
       </c>
-      <c r="L7" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="M7" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="N7" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O7" s="20" t="s">
+      <c r="L7" s="67" t="s">
+        <v>95</v>
+      </c>
+      <c r="M7" s="68" t="s">
+        <v>70</v>
+      </c>
+      <c r="N7" s="69" t="s">
         <v>85</v>
       </c>
+      <c r="O7" s="66" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="62"/>
+      <c r="B8" s="62"/>
+      <c r="C8" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" s="18">
+      <c r="D8" s="62" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="63">
         <v>8192</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="63">
         <f t="shared" si="0"/>
         <v>73728</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="63">
         <f t="shared" si="1"/>
         <v>81919</v>
       </c>
-      <c r="H8" s="26" t="str">
+      <c r="H8" s="64" t="str">
         <f t="shared" si="3"/>
         <v>12000</v>
       </c>
-      <c r="I8" s="27" t="str">
+      <c r="I8" s="65" t="str">
         <f t="shared" si="4"/>
         <v>13FFF</v>
       </c>
-      <c r="J8" s="20" t="str">
+      <c r="J8" s="66" t="str">
         <f t="shared" si="5"/>
         <v>000000010011111111111111</v>
       </c>
-      <c r="K8" s="20" t="str">
+      <c r="K8" s="66" t="str">
         <f t="shared" si="2"/>
         <v>000000010010000000000000</v>
       </c>
-      <c r="L8" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="M8" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="N8" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O8" s="20" t="s">
+      <c r="L8" s="67" t="s">
+        <v>95</v>
+      </c>
+      <c r="M8" s="68" t="s">
+        <v>70</v>
+      </c>
+      <c r="N8" s="69" t="s">
         <v>85</v>
       </c>
+      <c r="O8" s="66" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="E9" s="18">
+      <c r="A9" s="62"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="63">
         <v>8192</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="63">
         <f t="shared" si="0"/>
         <v>81920</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="63">
         <f t="shared" si="1"/>
         <v>90111</v>
       </c>
-      <c r="H9" s="26" t="str">
+      <c r="H9" s="64" t="str">
         <f t="shared" si="3"/>
         <v>14000</v>
       </c>
-      <c r="I9" s="27" t="str">
+      <c r="I9" s="65" t="str">
         <f t="shared" si="4"/>
         <v>15FFF</v>
       </c>
-      <c r="J9" s="20" t="str">
+      <c r="J9" s="66" t="str">
         <f t="shared" si="5"/>
         <v>000000010101111111111111</v>
       </c>
-      <c r="K9" s="20" t="str">
+      <c r="K9" s="66" t="str">
         <f t="shared" si="2"/>
         <v>000000010100000000000000</v>
       </c>
-      <c r="L9" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="M9" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="N9" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O9" s="20" t="s">
+      <c r="L9" s="67" t="s">
+        <v>95</v>
+      </c>
+      <c r="M9" s="68" t="s">
+        <v>70</v>
+      </c>
+      <c r="N9" s="69" t="s">
         <v>85</v>
       </c>
+      <c r="O9" s="66" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="E10" s="18">
+      <c r="A10" s="62"/>
+      <c r="B10" s="62"/>
+      <c r="C10" s="62" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="62" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="63">
         <v>8192</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="63">
         <f t="shared" si="0"/>
         <v>90112</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="63">
         <f t="shared" si="1"/>
         <v>98303</v>
       </c>
-      <c r="H10" s="26" t="str">
+      <c r="H10" s="64" t="str">
         <f t="shared" si="3"/>
         <v>16000</v>
       </c>
-      <c r="I10" s="27" t="str">
+      <c r="I10" s="65" t="str">
         <f t="shared" si="4"/>
         <v>17FFF</v>
       </c>
-      <c r="J10" s="20" t="str">
+      <c r="J10" s="66" t="str">
         <f t="shared" si="5"/>
         <v>000000010111111111111111</v>
       </c>
-      <c r="K10" s="20" t="str">
+      <c r="K10" s="66" t="str">
         <f t="shared" si="2"/>
         <v>000000010110000000000000</v>
       </c>
-      <c r="L10" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="M10" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="N10" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O10" s="20" t="s">
+      <c r="L10" s="67" t="s">
+        <v>95</v>
+      </c>
+      <c r="M10" s="68" t="s">
+        <v>70</v>
+      </c>
+      <c r="N10" s="69" t="s">
         <v>85</v>
       </c>
+      <c r="O10" s="66" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="E11" s="18">
+      <c r="A11" s="54"/>
+      <c r="B11" s="54" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="55">
         <v>8192</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="55">
         <f t="shared" si="0"/>
         <v>98304</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="55">
         <f t="shared" si="1"/>
         <v>106495</v>
       </c>
-      <c r="H11" s="26" t="str">
+      <c r="H11" s="56" t="str">
         <f t="shared" si="3"/>
         <v>18000</v>
       </c>
-      <c r="I11" s="27" t="str">
+      <c r="I11" s="57" t="str">
         <f t="shared" si="4"/>
         <v>19FFF</v>
       </c>
-      <c r="J11" s="20" t="str">
+      <c r="J11" s="58" t="str">
         <f t="shared" si="5"/>
         <v>000000011001111111111111</v>
       </c>
-      <c r="K11" s="20" t="str">
+      <c r="K11" s="58" t="str">
         <f t="shared" si="2"/>
         <v>000000011000000000000000</v>
       </c>
-      <c r="L11" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="M11" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="N11" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O11" s="20" t="s">
+      <c r="L11" s="59" t="s">
+        <v>95</v>
+      </c>
+      <c r="M11" s="60" t="s">
+        <v>75</v>
+      </c>
+      <c r="N11" s="61" t="s">
         <v>85</v>
       </c>
+      <c r="O11" s="58" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="E12" s="18">
+      <c r="A12" s="54"/>
+      <c r="B12" s="54"/>
+      <c r="C12" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="55">
         <v>8192</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="55">
         <f t="shared" si="0"/>
         <v>106496</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="55">
         <f t="shared" si="1"/>
         <v>114687</v>
       </c>
-      <c r="H12" s="26" t="str">
+      <c r="H12" s="56" t="str">
         <f t="shared" si="3"/>
         <v>1A000</v>
       </c>
-      <c r="I12" s="27" t="str">
+      <c r="I12" s="57" t="str">
         <f t="shared" si="4"/>
         <v>1BFFF</v>
       </c>
-      <c r="J12" s="20" t="str">
+      <c r="J12" s="58" t="str">
         <f t="shared" si="5"/>
         <v>000000011011111111111111</v>
       </c>
-      <c r="K12" s="20" t="str">
+      <c r="K12" s="58" t="str">
         <f t="shared" si="2"/>
         <v>000000011010000000000000</v>
       </c>
-      <c r="L12" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="M12" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="N12" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O12" s="20" t="s">
+      <c r="L12" s="59" t="s">
+        <v>95</v>
+      </c>
+      <c r="M12" s="60" t="s">
+        <v>75</v>
+      </c>
+      <c r="N12" s="61" t="s">
         <v>85</v>
       </c>
+      <c r="O12" s="58" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="E13" s="18">
+      <c r="A13" s="54"/>
+      <c r="B13" s="54"/>
+      <c r="C13" s="54" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="54" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="55">
         <v>8192</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="55">
         <f t="shared" si="0"/>
         <v>114688</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="55">
         <f t="shared" si="1"/>
         <v>122879</v>
       </c>
-      <c r="H13" s="26" t="str">
+      <c r="H13" s="56" t="str">
         <f t="shared" si="3"/>
         <v>1C000</v>
       </c>
-      <c r="I13" s="27" t="str">
+      <c r="I13" s="57" t="str">
         <f t="shared" si="4"/>
         <v>1DFFF</v>
       </c>
-      <c r="J13" s="20" t="str">
+      <c r="J13" s="58" t="str">
         <f t="shared" si="5"/>
         <v>000000011101111111111111</v>
       </c>
-      <c r="K13" s="20" t="str">
+      <c r="K13" s="58" t="str">
         <f t="shared" si="2"/>
         <v>000000011100000000000000</v>
       </c>
-      <c r="L13" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="M13" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="N13" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O13" s="20" t="s">
+      <c r="L13" s="59" t="s">
+        <v>95</v>
+      </c>
+      <c r="M13" s="60" t="s">
+        <v>75</v>
+      </c>
+      <c r="N13" s="61" t="s">
         <v>85</v>
       </c>
+      <c r="O13" s="58" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" s="18">
+      <c r="A14" s="54"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="54" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="55">
         <v>8192</v>
       </c>
-      <c r="F14" s="18">
+      <c r="F14" s="55">
         <f t="shared" si="0"/>
         <v>122880</v>
       </c>
-      <c r="G14" s="18">
+      <c r="G14" s="55">
         <f t="shared" si="1"/>
         <v>131071</v>
       </c>
-      <c r="H14" s="26" t="str">
+      <c r="H14" s="56" t="str">
         <f t="shared" si="3"/>
         <v>1E000</v>
       </c>
-      <c r="I14" s="27" t="str">
+      <c r="I14" s="57" t="str">
         <f t="shared" si="4"/>
         <v>1FFFF</v>
       </c>
-      <c r="J14" s="20" t="str">
+      <c r="J14" s="58" t="str">
         <f t="shared" si="5"/>
         <v>000000011111111111111111</v>
       </c>
-      <c r="K14" s="20" t="str">
+      <c r="K14" s="58" t="str">
         <f t="shared" si="2"/>
         <v>000000011110000000000000</v>
       </c>
-      <c r="L14" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="M14" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="N14" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O14" s="20" t="s">
+      <c r="L14" s="59" t="s">
+        <v>95</v>
+      </c>
+      <c r="M14" s="60" t="s">
+        <v>75</v>
+      </c>
+      <c r="N14" s="61" t="s">
         <v>85</v>
       </c>
+      <c r="O14" s="58" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" s="18">
+      <c r="A15" s="46"/>
+      <c r="B15" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="47">
         <v>8192</v>
       </c>
-      <c r="F15" s="18">
+      <c r="F15" s="47">
         <f t="shared" si="0"/>
         <v>131072</v>
       </c>
-      <c r="G15" s="18">
+      <c r="G15" s="47">
         <f t="shared" si="1"/>
         <v>139263</v>
       </c>
-      <c r="H15" s="26" t="str">
+      <c r="H15" s="48" t="str">
         <f t="shared" si="3"/>
         <v>20000</v>
       </c>
-      <c r="I15" s="27" t="str">
+      <c r="I15" s="49" t="str">
         <f t="shared" si="4"/>
         <v>21FFF</v>
       </c>
-      <c r="J15" s="20" t="str">
+      <c r="J15" s="50" t="str">
         <f t="shared" si="5"/>
         <v>000000100001111111111111</v>
       </c>
-      <c r="K15" s="20" t="str">
+      <c r="K15" s="50" t="str">
         <f t="shared" si="2"/>
         <v>000000100000000000000000</v>
       </c>
-      <c r="L15" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="M15" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="N15" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O15" s="20" t="s">
+      <c r="L15" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="M15" s="52" t="s">
+        <v>103</v>
+      </c>
+      <c r="N15" s="53" t="s">
         <v>85</v>
       </c>
+      <c r="O15" s="50" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="E16" s="18">
+      <c r="A16" s="46"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="47">
         <v>8192</v>
       </c>
-      <c r="F16" s="18">
+      <c r="F16" s="47">
         <f t="shared" si="0"/>
         <v>139264</v>
       </c>
-      <c r="G16" s="18">
+      <c r="G16" s="47">
         <f t="shared" si="1"/>
         <v>147455</v>
       </c>
-      <c r="H16" s="26" t="str">
+      <c r="H16" s="48" t="str">
         <f t="shared" si="3"/>
         <v>22000</v>
       </c>
-      <c r="I16" s="27" t="str">
+      <c r="I16" s="49" t="str">
         <f t="shared" si="4"/>
         <v>23FFF</v>
       </c>
-      <c r="J16" s="20" t="str">
+      <c r="J16" s="50" t="str">
         <f t="shared" si="5"/>
         <v>000000100011111111111111</v>
       </c>
-      <c r="K16" s="20" t="str">
+      <c r="K16" s="50" t="str">
         <f t="shared" si="2"/>
         <v>000000100010000000000000</v>
       </c>
-      <c r="L16" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="M16" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="N16" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O16" s="20" t="s">
+      <c r="L16" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="M16" s="52" t="s">
+        <v>103</v>
+      </c>
+      <c r="N16" s="53" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" s="18">
+      <c r="O16" s="50" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="46"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="47">
         <v>8192</v>
       </c>
-      <c r="F17" s="18">
+      <c r="F17" s="47">
         <f t="shared" si="0"/>
         <v>147456</v>
       </c>
-      <c r="G17" s="18">
+      <c r="G17" s="47">
         <f t="shared" si="1"/>
         <v>155647</v>
       </c>
-      <c r="H17" s="26" t="str">
+      <c r="H17" s="48" t="str">
         <f t="shared" si="3"/>
         <v>24000</v>
       </c>
-      <c r="I17" s="27" t="str">
+      <c r="I17" s="49" t="str">
         <f t="shared" si="4"/>
         <v>25FFF</v>
       </c>
-      <c r="J17" s="20" t="str">
+      <c r="J17" s="50" t="str">
         <f t="shared" si="5"/>
         <v>000000100101111111111111</v>
       </c>
-      <c r="K17" s="20" t="str">
+      <c r="K17" s="50" t="str">
         <f t="shared" si="2"/>
         <v>000000100100000000000000</v>
       </c>
-      <c r="L17" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="M17" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="N17" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O17" s="20" t="s">
+      <c r="L17" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="M17" s="52" t="s">
+        <v>103</v>
+      </c>
+      <c r="N17" s="53" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" s="18">
+      <c r="O17" s="50" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="46"/>
+      <c r="B18" s="46"/>
+      <c r="C18" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="47">
         <v>8192</v>
       </c>
-      <c r="F18" s="18">
+      <c r="F18" s="47">
         <f t="shared" si="0"/>
         <v>155648</v>
       </c>
-      <c r="G18" s="18">
+      <c r="G18" s="47">
         <f t="shared" si="1"/>
         <v>163839</v>
       </c>
-      <c r="H18" s="26" t="str">
+      <c r="H18" s="48" t="str">
         <f t="shared" si="3"/>
         <v>26000</v>
       </c>
-      <c r="I18" s="27" t="str">
+      <c r="I18" s="49" t="str">
         <f t="shared" si="4"/>
         <v>27FFF</v>
       </c>
-      <c r="J18" s="20" t="str">
+      <c r="J18" s="50" t="str">
         <f t="shared" si="5"/>
         <v>000000100111111111111111</v>
       </c>
-      <c r="K18" s="20" t="str">
+      <c r="K18" s="50" t="str">
         <f t="shared" si="2"/>
         <v>000000100110000000000000</v>
       </c>
-      <c r="L18" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="M18" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="N18" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O18" s="20" t="s">
+      <c r="L18" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="M18" s="52" t="s">
+        <v>103</v>
+      </c>
+      <c r="N18" s="53" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="E19" s="18">
+      <c r="O18" s="50" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="37"/>
+      <c r="B19" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="38">
         <v>8192</v>
       </c>
-      <c r="F19" s="18">
+      <c r="F19" s="38">
         <f t="shared" si="0"/>
         <v>163840</v>
       </c>
-      <c r="G19" s="18">
+      <c r="G19" s="38">
         <f t="shared" si="1"/>
         <v>172031</v>
       </c>
-      <c r="H19" s="26" t="str">
+      <c r="H19" s="39" t="str">
         <f t="shared" si="3"/>
         <v>28000</v>
       </c>
-      <c r="I19" s="27" t="str">
+      <c r="I19" s="40" t="str">
         <f t="shared" si="4"/>
         <v>29FFF</v>
       </c>
-      <c r="J19" s="20" t="str">
+      <c r="J19" s="41" t="str">
         <f t="shared" si="5"/>
         <v>000000101001111111111111</v>
       </c>
-      <c r="K19" s="20" t="str">
+      <c r="K19" s="41" t="str">
         <f t="shared" si="2"/>
         <v>000000101000000000000000</v>
       </c>
-      <c r="L19" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="M19" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="N19" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O19" s="20" t="s">
+      <c r="L19" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="M19" s="43" t="s">
+        <v>104</v>
+      </c>
+      <c r="N19" s="44" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="E20" s="18">
+      <c r="O19" s="41" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="37"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="38">
         <v>8192</v>
       </c>
-      <c r="F20" s="18">
+      <c r="F20" s="38">
         <f t="shared" si="0"/>
         <v>172032</v>
       </c>
-      <c r="G20" s="18">
+      <c r="G20" s="38">
         <f t="shared" si="1"/>
         <v>180223</v>
       </c>
-      <c r="H20" s="26" t="str">
+      <c r="H20" s="39" t="str">
         <f t="shared" si="3"/>
         <v>2A000</v>
       </c>
-      <c r="I20" s="27" t="str">
+      <c r="I20" s="40" t="str">
         <f t="shared" si="4"/>
         <v>2BFFF</v>
       </c>
-      <c r="J20" s="20" t="str">
+      <c r="J20" s="41" t="str">
         <f t="shared" si="5"/>
         <v>000000101011111111111111</v>
       </c>
-      <c r="K20" s="20" t="str">
+      <c r="K20" s="41" t="str">
         <f t="shared" si="2"/>
         <v>000000101010000000000000</v>
       </c>
-      <c r="L20" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="M20" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="N20" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O20" s="20" t="s">
+      <c r="L20" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="M20" s="43" t="s">
+        <v>104</v>
+      </c>
+      <c r="N20" s="44" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="E21" s="18">
+      <c r="O20" s="41" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="37"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" s="38">
         <v>8192</v>
       </c>
-      <c r="F21" s="18">
+      <c r="F21" s="38">
         <f t="shared" si="0"/>
         <v>180224</v>
       </c>
-      <c r="G21" s="18">
+      <c r="G21" s="38">
         <f t="shared" si="1"/>
         <v>188415</v>
       </c>
-      <c r="H21" s="26" t="str">
+      <c r="H21" s="39" t="str">
         <f t="shared" si="3"/>
         <v>2C000</v>
       </c>
-      <c r="I21" s="27" t="str">
+      <c r="I21" s="40" t="str">
         <f t="shared" si="4"/>
         <v>2DFFF</v>
       </c>
-      <c r="J21" s="20" t="str">
+      <c r="J21" s="41" t="str">
         <f t="shared" si="5"/>
         <v>000000101101111111111111</v>
       </c>
-      <c r="K21" s="20" t="str">
+      <c r="K21" s="41" t="str">
         <f t="shared" si="2"/>
         <v>000000101100000000000000</v>
       </c>
-      <c r="L21" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="M21" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="N21" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O21" s="20" t="s">
+      <c r="L21" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="M21" s="43" t="s">
+        <v>104</v>
+      </c>
+      <c r="N21" s="44" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="C22" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="D22" s="23"/>
-      <c r="E22" s="18">
+      <c r="O21" s="41" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="37"/>
+      <c r="B22" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="45"/>
+      <c r="E22" s="38">
         <v>8192</v>
       </c>
-      <c r="F22" s="18">
+      <c r="F22" s="38">
         <f t="shared" si="0"/>
         <v>188416</v>
       </c>
-      <c r="G22" s="18">
+      <c r="G22" s="38">
         <f t="shared" si="1"/>
         <v>196607</v>
       </c>
-      <c r="H22" s="26" t="str">
+      <c r="H22" s="39" t="str">
         <f t="shared" si="3"/>
         <v>2E000</v>
       </c>
-      <c r="I22" s="27" t="str">
+      <c r="I22" s="40" t="str">
         <f t="shared" si="4"/>
         <v>2FFFF</v>
       </c>
-      <c r="J22" s="20" t="str">
+      <c r="J22" s="41" t="str">
         <f t="shared" si="5"/>
         <v>000000101111111111111111</v>
       </c>
-      <c r="K22" s="20" t="str">
+      <c r="K22" s="41" t="str">
         <f t="shared" si="2"/>
         <v>000000101110000000000000</v>
       </c>
-      <c r="L22" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="M22" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="N22" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O22" s="20" t="s">
+      <c r="L22" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="M22" s="43" t="s">
+        <v>104</v>
+      </c>
+      <c r="N22" s="44" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="O22" s="41" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
       <c r="B23" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>51</v>
+        <v>112</v>
+      </c>
+      <c r="C23" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>91</v>
       </c>
       <c r="E23" s="18">
-        <v>4096</v>
+        <v>32768</v>
       </c>
       <c r="F23" s="18">
         <f t="shared" si="0"/>
@@ -1956,7 +2045,7 @@
       </c>
       <c r="G23" s="18">
         <f t="shared" si="1"/>
-        <v>200703</v>
+        <v>229375</v>
       </c>
       <c r="H23" s="26" t="str">
         <f t="shared" si="3"/>
@@ -1964,398 +2053,377 @@
       </c>
       <c r="I23" s="27" t="str">
         <f t="shared" si="4"/>
-        <v>30FFF</v>
+        <v>37FFF</v>
       </c>
       <c r="J23" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>000000110000111111111111</v>
+        <v>000000110111111111111111</v>
       </c>
       <c r="K23" s="20" t="str">
         <f t="shared" si="2"/>
         <v>000000110000000000000000</v>
       </c>
       <c r="L23" s="21" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="M23" s="22" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="N23" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="O23" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="P23" s="1" t="s">
+      <c r="O23" s="20"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+      <c r="B24" s="17" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>52</v>
+      <c r="C24" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>92</v>
       </c>
       <c r="E24" s="18">
-        <v>4096</v>
+        <v>32768</v>
       </c>
       <c r="F24" s="18">
         <f t="shared" si="0"/>
-        <v>200704</v>
+        <v>229376</v>
       </c>
       <c r="G24" s="18">
         <f t="shared" si="1"/>
-        <v>204799</v>
+        <v>262143</v>
       </c>
       <c r="H24" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>31000</v>
+        <v>38000</v>
       </c>
       <c r="I24" s="27" t="str">
         <f t="shared" si="4"/>
-        <v>31FFF</v>
+        <v>3FFFF</v>
       </c>
       <c r="J24" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>000000110001111111111111</v>
+        <v>000000111111111111111111</v>
       </c>
       <c r="K24" s="20" t="str">
         <f t="shared" si="2"/>
-        <v>000000110001000000000000</v>
+        <v>000000111000000000000000</v>
       </c>
       <c r="L24" s="21" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="M24" s="22" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="N24" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="O24" s="20" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O24" s="20"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="D25" s="17"/>
+        <v>114</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>93</v>
+      </c>
       <c r="E25" s="18">
-        <v>16384</v>
+        <v>32768</v>
       </c>
       <c r="F25" s="18">
         <f t="shared" si="0"/>
-        <v>204800</v>
+        <v>262144</v>
       </c>
       <c r="G25" s="18">
         <f t="shared" si="1"/>
-        <v>221183</v>
+        <v>294911</v>
       </c>
       <c r="H25" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>32000</v>
+        <v>40000</v>
       </c>
       <c r="I25" s="27" t="str">
         <f t="shared" si="4"/>
-        <v>35FFF</v>
+        <v>47FFF</v>
       </c>
       <c r="J25" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>000000110101111111111111</v>
+        <v>000001000111111111111111</v>
       </c>
       <c r="K25" s="20" t="str">
         <f t="shared" si="2"/>
-        <v>000000110010000000000000</v>
+        <v>000001000000000000000000</v>
       </c>
       <c r="L25" s="21" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="M25" s="22" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="N25" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="O25" s="20" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="O25" s="20"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="29"/>
+      <c r="B26" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="E26" s="18">
+      <c r="D26" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" s="30">
+        <v>4096</v>
+      </c>
+      <c r="F26" s="30">
+        <f t="shared" si="0"/>
+        <v>294912</v>
+      </c>
+      <c r="G26" s="30">
+        <f t="shared" si="1"/>
+        <v>299007</v>
+      </c>
+      <c r="H26" s="31" t="str">
+        <f t="shared" si="3"/>
+        <v>48000</v>
+      </c>
+      <c r="I26" s="32" t="str">
+        <f t="shared" si="4"/>
+        <v>48FFF</v>
+      </c>
+      <c r="J26" s="33" t="str">
+        <f t="shared" si="5"/>
+        <v>000001001000111111111111</v>
+      </c>
+      <c r="K26" s="33" t="str">
+        <f t="shared" si="2"/>
+        <v>000001001000000000000000</v>
+      </c>
+      <c r="L26" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="M26" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="N26" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="O26" s="33"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="29"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="E27" s="30">
+        <v>4096</v>
+      </c>
+      <c r="F27" s="30">
+        <f t="shared" si="0"/>
+        <v>299008</v>
+      </c>
+      <c r="G27" s="30">
+        <f t="shared" si="1"/>
+        <v>303103</v>
+      </c>
+      <c r="H27" s="31" t="str">
+        <f t="shared" si="3"/>
+        <v>49000</v>
+      </c>
+      <c r="I27" s="32" t="str">
+        <f t="shared" si="4"/>
+        <v>49FFF</v>
+      </c>
+      <c r="J27" s="33" t="str">
+        <f t="shared" si="5"/>
+        <v>000001001001111111111111</v>
+      </c>
+      <c r="K27" s="33" t="str">
+        <f t="shared" si="2"/>
+        <v>000001001001000000000000</v>
+      </c>
+      <c r="L27" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="M27" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="N27" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="O27" s="33"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" s="18">
         <v>8192</v>
-      </c>
-      <c r="F26" s="18">
-        <f t="shared" si="0"/>
-        <v>221184</v>
-      </c>
-      <c r="G26" s="18">
-        <f t="shared" si="1"/>
-        <v>229375</v>
-      </c>
-      <c r="H26" s="26" t="str">
-        <f t="shared" si="3"/>
-        <v>36000</v>
-      </c>
-      <c r="I26" s="27" t="str">
-        <f t="shared" si="4"/>
-        <v>37FFF</v>
-      </c>
-      <c r="J26" s="20" t="str">
-        <f t="shared" si="5"/>
-        <v>000000110111111111111111</v>
-      </c>
-      <c r="K26" s="20" t="str">
-        <f t="shared" si="2"/>
-        <v>000000110110000000000000</v>
-      </c>
-      <c r="L26" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="M26" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="N26" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="O26" s="20" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="D27" s="17"/>
-      <c r="E27" s="18">
-        <v>20480</v>
-      </c>
-      <c r="F27" s="18">
-        <f t="shared" si="0"/>
-        <v>229376</v>
-      </c>
-      <c r="G27" s="18">
-        <f t="shared" si="1"/>
-        <v>249855</v>
-      </c>
-      <c r="H27" s="26" t="str">
-        <f t="shared" si="3"/>
-        <v>38000</v>
-      </c>
-      <c r="I27" s="27" t="str">
-        <f t="shared" si="4"/>
-        <v>3CFFF</v>
-      </c>
-      <c r="J27" s="20" t="str">
-        <f t="shared" si="5"/>
-        <v>000000111100111111111111</v>
-      </c>
-      <c r="K27" s="20" t="str">
-        <f t="shared" si="2"/>
-        <v>000000111000000000000000</v>
-      </c>
-      <c r="L27" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="M27" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="N27" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="O27" s="20" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="E28" s="18">
-        <v>4096</v>
       </c>
       <c r="F28" s="18">
         <f t="shared" si="0"/>
-        <v>249856</v>
+        <v>303104</v>
       </c>
       <c r="G28" s="18">
         <f t="shared" si="1"/>
-        <v>253951</v>
+        <v>311295</v>
       </c>
       <c r="H28" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>3D000</v>
+        <v>4A000</v>
       </c>
       <c r="I28" s="27" t="str">
         <f t="shared" si="4"/>
-        <v>3DFFF</v>
+        <v>4BFFF</v>
       </c>
       <c r="J28" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>000000111101111111111111</v>
+        <v>000001001011111111111111</v>
       </c>
       <c r="K28" s="20" t="str">
         <f t="shared" si="2"/>
-        <v>000000111101000000000000</v>
+        <v>000001001010000000000000</v>
       </c>
       <c r="L28" s="21" t="s">
-        <v>74</v>
+        <v>105</v>
       </c>
       <c r="M28" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N28" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="O28" s="20" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="O28" s="20"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="17" t="s">
-        <v>101</v>
+        <v>31</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="D29" s="17"/>
+        <v>32</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>45</v>
+      </c>
       <c r="E29" s="18">
         <v>4096</v>
       </c>
       <c r="F29" s="18">
         <f t="shared" si="0"/>
-        <v>253952</v>
+        <v>311296</v>
       </c>
       <c r="G29" s="18">
         <f t="shared" si="1"/>
-        <v>258047</v>
+        <v>315391</v>
       </c>
       <c r="H29" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>3E000</v>
+        <v>4C000</v>
       </c>
       <c r="I29" s="27" t="str">
         <f t="shared" si="4"/>
-        <v>3EFFF</v>
+        <v>4CFFF</v>
       </c>
       <c r="J29" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>000000111110111111111111</v>
+        <v>000001001100111111111111</v>
       </c>
       <c r="K29" s="20" t="str">
         <f t="shared" si="2"/>
-        <v>000000111110000000000000</v>
+        <v>000001001100000000000000</v>
       </c>
       <c r="L29" s="21" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="M29" s="22" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="N29" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="O29" s="20" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
-        <v>42</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="O29" s="20"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="8"/>
       <c r="B30" s="19" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E30" s="18">
         <v>512</v>
       </c>
       <c r="F30" s="18">
         <f t="shared" si="0"/>
-        <v>258048</v>
+        <v>315392</v>
       </c>
       <c r="G30" s="18">
         <f t="shared" si="1"/>
-        <v>258559</v>
+        <v>315903</v>
       </c>
       <c r="H30" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>3F000</v>
+        <v>4D000</v>
       </c>
       <c r="I30" s="27" t="str">
         <f t="shared" si="4"/>
-        <v>3F1FF</v>
+        <v>4D1FF</v>
       </c>
       <c r="J30" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>000000111111000111111111</v>
+        <v>000001001101000111111111</v>
       </c>
       <c r="K30" s="20" t="str">
         <f t="shared" si="2"/>
-        <v>000000111111000000000000</v>
+        <v>000001001101000000000000</v>
       </c>
       <c r="L30" s="21" t="s">
-        <v>81</v>
+        <v>107</v>
       </c>
       <c r="M30" s="22" t="s">
         <v>111</v>
       </c>
       <c r="N30" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="O30" s="20" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="O30" s="20"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="10">
@@ -2364,73 +2432,28 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D33" s="9"/>
       <c r="E33" s="10">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D34" s="9"/>
-      <c r="E34" s="10">
-        <v>32768</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D35" s="9"/>
-      <c r="E35" s="10">
-        <v>32768</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D36" s="9"/>
-      <c r="E36" s="10">
-        <v>32768</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="D23:D30 D3:D21">
-    <cfRule type="duplicateValues" dxfId="2" priority="25"/>
+  <conditionalFormatting sqref="D26:D30 D3:D21">
+    <cfRule type="duplicateValues" dxfId="2" priority="74"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J30">
-    <cfRule type="duplicateValues" dxfId="1" priority="59"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="77"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K30">
-    <cfRule type="duplicateValues" dxfId="0" priority="61"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="79"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2454,7 +2477,7 @@
   <sheetData>
     <row r="1" spans="1:25" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B1" s="25">
         <v>23</v>
@@ -2531,7 +2554,7 @@
     </row>
     <row r="2" spans="1:25" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="24" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B2" s="25">
         <f>2^24</f>

</xml_diff>

<commit_message>
update layout and MRA for sound board
</commit_message>
<xml_diff>
--- a/doc/rom_calc_joust2.xlsx
+++ b/doc/rom_calc_joust2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kcoleman\Documents\GitHub\Arcade-Joust2_MiSTer\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00F1364-2A3A-4697-820F-ED052395E303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243FCCEF-168E-469A-B833-9703551338FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-14550" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="116">
   <si>
     <t>section</t>
   </si>
@@ -367,9 +367,6 @@
     <t>100110</t>
   </si>
   <si>
-    <t>1001101000</t>
-  </si>
-  <si>
     <t>sound_bank_a</t>
   </si>
   <si>
@@ -377,6 +374,12 @@
   </si>
   <si>
     <t>sound_bank_c</t>
+  </si>
+  <si>
+    <t>100111</t>
+  </si>
+  <si>
+    <t>1010000000</t>
   </si>
 </sst>
 </file>
@@ -946,10 +949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47A4B22B-6618-4C49-8781-19881A3A2D30}">
-  <dimension ref="A1:O33"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:O30"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -1046,11 +1049,11 @@
         <v>16384</v>
       </c>
       <c r="F3" s="18">
-        <f t="shared" ref="F3:F30" si="0">E2+F2</f>
+        <f t="shared" ref="F3:F31" si="0">E2+F2</f>
         <v>0</v>
       </c>
       <c r="G3" s="18">
-        <f t="shared" ref="G3:G30" si="1">E3+F3-1</f>
+        <f t="shared" ref="G3:G31" si="1">E3+F3-1</f>
         <v>16383</v>
       </c>
       <c r="H3" s="26" t="str">
@@ -1066,7 +1069,7 @@
         <v>000000000011111111111111</v>
       </c>
       <c r="K3" s="20" t="str">
-        <f t="shared" ref="K3:K30" si="2">DEC2BIN(MOD(QUOTIENT($F3,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F3,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F3,256^0),256),8)</f>
+        <f t="shared" ref="K3:K31" si="2">DEC2BIN(MOD(QUOTIENT($F3,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F3,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F3,256^0),256),8)</f>
         <v>000000000000000000000000</v>
       </c>
       <c r="L3" s="21" t="s">
@@ -1105,15 +1108,15 @@
         <v>32767</v>
       </c>
       <c r="H4" s="26" t="str">
-        <f t="shared" ref="H4:H30" si="3">DEC2HEX(E3+F3,5)</f>
+        <f t="shared" ref="H4:H31" si="3">DEC2HEX(E3+F3,5)</f>
         <v>04000</v>
       </c>
       <c r="I4" s="27" t="str">
-        <f t="shared" ref="I4:I30" si="4">DEC2HEX(E4+F4-1,5)</f>
+        <f t="shared" ref="I4:I31" si="4">DEC2HEX(E4+F4-1,5)</f>
         <v>07FFF</v>
       </c>
       <c r="J4" s="20" t="str">
-        <f t="shared" ref="J4:J30" si="5">DEC2BIN(MOD(QUOTIENT($G4,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($G4,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($G4,256^0),256),8)</f>
+        <f t="shared" ref="J4:J31" si="5">DEC2BIN(MOD(QUOTIENT($G4,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($G4,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($G4,256^0),256),8)</f>
         <v>000000000111111111111111</v>
       </c>
       <c r="K4" s="20" t="str">
@@ -2028,7 +2031,7 @@
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C23" s="23" t="s">
         <v>42</v>
@@ -2077,7 +2080,7 @@
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C24" s="23" t="s">
         <v>43</v>
@@ -2126,7 +2129,7 @@
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C25" s="23" t="s">
         <v>44</v>
@@ -2320,16 +2323,14 @@
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="17" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D29" s="17" t="s">
-        <v>45</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="D29" s="17"/>
       <c r="E29" s="18">
-        <v>4096</v>
+        <v>12288</v>
       </c>
       <c r="F29" s="18">
         <f t="shared" si="0"/>
@@ -2337,7 +2338,7 @@
       </c>
       <c r="G29" s="18">
         <f t="shared" si="1"/>
-        <v>315391</v>
+        <v>323583</v>
       </c>
       <c r="H29" s="26" t="str">
         <f t="shared" si="3"/>
@@ -2345,90 +2346,124 @@
       </c>
       <c r="I29" s="27" t="str">
         <f t="shared" si="4"/>
-        <v>4CFFF</v>
+        <v>4EFFF</v>
       </c>
       <c r="J29" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>000001001100111111111111</v>
+        <v>000001001110111111111111</v>
       </c>
       <c r="K29" s="20" t="str">
         <f t="shared" si="2"/>
         <v>000001001100000000000000</v>
       </c>
       <c r="L29" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M29" s="22" t="s">
         <v>110</v>
       </c>
       <c r="N29" s="28" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="O29" s="20"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
-      <c r="B30" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="19" t="s">
-        <v>37</v>
+      <c r="A30" s="7"/>
+      <c r="B30" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>32</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="E30" s="18">
-        <v>512</v>
+        <v>4096</v>
       </c>
       <c r="F30" s="18">
         <f t="shared" si="0"/>
-        <v>315392</v>
+        <v>323584</v>
       </c>
       <c r="G30" s="18">
         <f t="shared" si="1"/>
-        <v>315903</v>
+        <v>327679</v>
       </c>
       <c r="H30" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>4D000</v>
+        <v>4F000</v>
       </c>
       <c r="I30" s="27" t="str">
         <f t="shared" si="4"/>
-        <v>4D1FF</v>
+        <v>4FFFF</v>
       </c>
       <c r="J30" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>000001001101000111111111</v>
+        <v>000001001111111111111111</v>
       </c>
       <c r="K30" s="20" t="str">
         <f t="shared" si="2"/>
-        <v>000001001101000000000000</v>
+        <v>000001001111000000000000</v>
       </c>
       <c r="L30" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="M30" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="N30" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="O30" s="20"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="8"/>
+      <c r="B31" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" s="18">
+        <v>512</v>
+      </c>
+      <c r="F31" s="18">
+        <f t="shared" si="0"/>
+        <v>327680</v>
+      </c>
+      <c r="G31" s="18">
+        <f t="shared" si="1"/>
+        <v>328191</v>
+      </c>
+      <c r="H31" s="26" t="str">
+        <f t="shared" si="3"/>
+        <v>50000</v>
+      </c>
+      <c r="I31" s="27" t="str">
+        <f t="shared" si="4"/>
+        <v>501FF</v>
+      </c>
+      <c r="J31" s="20" t="str">
+        <f t="shared" si="5"/>
+        <v>000001010000000111111111</v>
+      </c>
+      <c r="K31" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>000001010000000000000000</v>
+      </c>
+      <c r="L31" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="M30" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="N30" s="28" t="s">
+      <c r="M31" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="N31" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="O30" s="20"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D32" s="9"/>
-      <c r="E32" s="10">
-        <v>256</v>
-      </c>
+      <c r="O31" s="20"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
@@ -2438,22 +2473,37 @@
         <v>39</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D33" s="9"/>
       <c r="E33" s="10">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" s="9"/>
+      <c r="E34" s="10">
         <v>32</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D26:D30 D3:D21">
-    <cfRule type="duplicateValues" dxfId="2" priority="74"/>
+  <conditionalFormatting sqref="D26:D31 D3:D21">
+    <cfRule type="duplicateValues" dxfId="2" priority="80"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J30">
-    <cfRule type="duplicateValues" dxfId="1" priority="77"/>
+  <conditionalFormatting sqref="J3:J31">
+    <cfRule type="duplicateValues" dxfId="1" priority="83"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K30">
-    <cfRule type="duplicateValues" dxfId="0" priority="79"/>
+  <conditionalFormatting sqref="K3:K31">
+    <cfRule type="duplicateValues" dxfId="0" priority="85"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>